<commit_message>
Adding extent report and log file
</commit_message>
<xml_diff>
--- a/testData/userTestData.xlsx
+++ b/testData/userTestData.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="21885" windowHeight="11100"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="12615" windowHeight="10920"/>
   </bookViews>
   <sheets>
-    <sheet name="userData" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:F16"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>username</t>
   </si>
@@ -40,9 +40,6 @@
     <t>rishov0514</t>
   </si>
   <si>
-    <t>Sj=hovik</t>
-  </si>
-  <si>
     <t>rdijsns@yahoo.com</t>
   </si>
   <si>
@@ -97,53 +94,53 @@
     <t>KiGunhh</t>
   </si>
   <si>
-    <t>rishov0515</t>
-  </si>
-  <si>
-    <t>rishov0516</t>
-  </si>
-  <si>
     <t>rishov0517</t>
   </si>
   <si>
-    <t>rishov0518</t>
-  </si>
-  <si>
-    <t>rishov0519</t>
-  </si>
-  <si>
-    <t>rishov0520</t>
-  </si>
-  <si>
-    <t>_001</t>
-  </si>
-  <si>
-    <t>_002</t>
-  </si>
-  <si>
-    <t>_003</t>
-  </si>
-  <si>
-    <t>_004</t>
-  </si>
-  <si>
-    <t>_005</t>
-  </si>
-  <si>
-    <t>_006</t>
-  </si>
-  <si>
-    <t>_007</t>
-  </si>
-  <si>
-    <t>UserId</t>
+    <t>Shovik</t>
+  </si>
+  <si>
+    <t>User_Id</t>
+  </si>
+  <si>
+    <t>rtyhov0515</t>
+  </si>
+  <si>
+    <t>bhgtv0518</t>
+  </si>
+  <si>
+    <t>kiuyov0516</t>
+  </si>
+  <si>
+    <t>lkkuy0519</t>
+  </si>
+  <si>
+    <t>aqwd0520</t>
+  </si>
+  <si>
+    <t>Kimberly</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>Larkin</t>
+  </si>
+  <si>
+    <t>Khan</t>
+  </si>
+  <si>
+    <t>Mia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,25 +155,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -188,21 +173,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Good" xfId="2" builtinId="26"/>
+  <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -498,212 +485,204 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="1" max="4" width="13.28515625" style="1"/>
+    <col min="5" max="5" width="21.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="13.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="1">
+        <v>1001</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" t="s">
+      <c r="A3" s="1">
+        <v>1002</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
+      <c r="F3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" t="s">
+      <c r="A4" s="1">
+        <v>1003</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" t="s">
+      <c r="A5" s="1">
+        <v>1004</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
+      <c r="F5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" t="s">
+      <c r="A6" s="1">
+        <v>1005</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
+      <c r="F6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" t="s">
+      <c r="A7" s="1">
+        <v>1006</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" t="s">
-        <v>11</v>
+      <c r="F7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" t="s">
+      <c r="A8" s="1">
+        <v>1007</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" t="s">
-        <v>12</v>
+      <c r="F8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
     <hyperlink ref="E3:E8" r:id="rId2" display="rdijsns@yahoo.com"/>

</xml_diff>